<commit_message>
feat: beep on fulfilled condition
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -11,15 +11,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>person</t>
   </si>
   <si>
+    <t>человек</t>
+  </si>
+  <si>
     <t>car</t>
   </si>
   <si>
+    <t>машина</t>
+  </si>
+  <si>
     <t>truck</t>
+  </si>
+  <si>
+    <t>грузовик</t>
   </si>
 </sst>
 </file>
@@ -283,20 +292,25 @@
       <c r="B1" s="1">
         <v>1.0</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2.0</v>
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>